<commit_message>
#Complite Excel Import & Configur Logging Pattern
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/supps_heet/supplier sheet.xlsx
+++ b/src/main/webapp/resources/supps_heet/supplier sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Ajith Motors</t>
   </si>
@@ -38,10 +38,37 @@
     <t>Kaml Bar</t>
   </si>
   <si>
-    <t>No 2/25 Arangala,Naula</t>
-  </si>
-  <si>
     <t>gdp@gmail.com</t>
+  </si>
+  <si>
+    <t>No 2/211 Arangala,Naula</t>
+  </si>
+  <si>
+    <t>Arpico PLC</t>
+  </si>
+  <si>
+    <t>No 3/14,Navinna,Colombo 3</t>
+  </si>
+  <si>
+    <t>arpico@gmail.com</t>
+  </si>
+  <si>
+    <t>Zloan PLC</t>
+  </si>
+  <si>
+    <t>No 11, Kadawatha,balummahara.</t>
+  </si>
+  <si>
+    <t>zloan@gmail.com</t>
+  </si>
+  <si>
+    <t>mitsui cement cop</t>
+  </si>
+  <si>
+    <t>No 32,Trnkomalee ,Kanthale</t>
+  </si>
+  <si>
+    <t>mit@yahoomail.com</t>
   </si>
 </sst>
 </file>
@@ -370,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,7 +434,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>726373936</v>
@@ -416,13 +443,67 @@
         <v>815683902</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>762561253</v>
+      </c>
+      <c r="D3">
+        <v>111459823</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>456259635</v>
+      </c>
+      <c r="D4">
+        <v>385215632</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>159632575</v>
+      </c>
+      <c r="D5">
+        <v>253974102</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E1" r:id="rId1"/>
     <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="E5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>